<commit_message>
move global parameters to logging
</commit_message>
<xml_diff>
--- a/experiments/20-01-22_15-22-34_all-cons.xlsx
+++ b/experiments/20-01-22_15-22-34_all-cons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yijiangh\Documents\pb_ws\pb-construction\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6899CA-140A-4697-A41E-25AD4941592C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323C4491-FCDC-43C5-80B4-66BA845A8E2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5072" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="103">
   <si>
     <t>config_id</t>
   </si>
@@ -328,12 +328,15 @@
   <si>
     <t>why does progression family completely fail here?</t>
   </si>
+  <si>
+    <t>Dijkstra: The two long cables keep coming back to the queue at the beginning of the search, while z will defer it</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,8 +364,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +393,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -410,12 +425,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -432,9 +448,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -738,14 +756,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="G219" sqref="G219"/>
+    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
+      <selection activeCell="K493" sqref="K493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="30.88671875" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -6269,7 +6288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -6322,26 +6341,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>129</v>
       </c>
       <c r="B131">
         <v>8</v>
       </c>
-      <c r="C131" s="3" t="s">
+      <c r="C131" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D131" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -6349,7 +6368,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -6399,7 +6418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -6452,7 +6471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -6505,7 +6524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -6558,7 +6577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -6611,7 +6630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -6663,8 +6682,11 @@
       <c r="S138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U138" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -6711,7 +6733,7 @@
         <v>373.5</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -6764,7 +6786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5">
         <v>139</v>
       </c>
@@ -6817,7 +6839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -6870,7 +6892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -6923,7 +6945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -7041,7 +7063,7 @@
       <c r="B147">
         <v>9</v>
       </c>
-      <c r="C147" s="3" t="s">
+      <c r="C147" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D147" t="s">
@@ -22211,7 +22233,7 @@
       <c r="B499">
         <v>31</v>
       </c>
-      <c r="C499" t="s">
+      <c r="C499" s="3" t="s">
         <v>83</v>
       </c>
       <c r="D499" t="s">
@@ -22900,7 +22922,7 @@
       <c r="B515">
         <v>32</v>
       </c>
-      <c r="C515" t="s">
+      <c r="C515" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D515" t="s">
@@ -24278,7 +24300,7 @@
       <c r="B547">
         <v>34</v>
       </c>
-      <c r="C547" t="s">
+      <c r="C547" s="3" t="s">
         <v>89</v>
       </c>
       <c r="D547" t="s">
@@ -24949,7 +24971,7 @@
       <c r="B563">
         <v>35</v>
       </c>
-      <c r="C563" t="s">
+      <c r="C563" s="3" t="s">
         <v>91</v>
       </c>
       <c r="D563" t="s">
@@ -26950,7 +26972,7 @@
       <c r="B611">
         <v>38</v>
       </c>
-      <c r="C611" t="s">
+      <c r="C611" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D611" t="s">
@@ -27633,7 +27655,7 @@
       <c r="B627">
         <v>39</v>
       </c>
-      <c r="C627" t="s">
+      <c r="C627" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D627" t="s">

</xml_diff>

<commit_message>
unite log and result dict keys and video saving (:cheers:)
</commit_message>
<xml_diff>
--- a/experiments/20-01-22_15-22-34_all-cons.xlsx
+++ b/experiments/20-01-22_15-22-34_all-cons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yijiangh\Documents\pb_ws\pb-construction\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323C4491-FCDC-43C5-80B4-66BA845A8E2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08035EB4-A8E9-4DFB-96D4-F1431CD88BE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4422" uniqueCount="103">
   <si>
     <t>config_id</t>
   </si>
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
-      <selection activeCell="K493" sqref="K493"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="H217" sqref="H217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10381,10 +10381,10 @@
       <c r="E225" t="s">
         <v>29</v>
       </c>
-      <c r="F225" t="s">
+      <c r="F225" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G225">
+      <c r="G225" s="6">
         <v>75</v>
       </c>
       <c r="H225">
@@ -26914,13 +26914,13 @@
       <c r="B609">
         <v>11</v>
       </c>
-      <c r="E609" t="s">
+      <c r="E609" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F609" t="s">
+      <c r="F609" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G609">
+      <c r="G609" s="6">
         <v>75</v>
       </c>
       <c r="H609">

</xml_diff>

<commit_message>
delete log exporting when plan is found
</commit_message>
<xml_diff>
--- a/experiments/20-01-22_15-22-34_all-cons.xlsx
+++ b/experiments/20-01-22_15-22-34_all-cons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yijiangh\Documents\pb_ws\pb-construction\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF07FB81-8BD9-4B06-8466-EE5AE4526D63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6618C8-F8A0-42D2-BB4C-2FED26027A47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4690" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="105">
   <si>
     <t>config_id</t>
   </si>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A474" workbookViewId="0">
-      <selection activeCell="G488" sqref="G488"/>
+    <sheetView tabSelected="1" topLeftCell="A471" workbookViewId="0">
+      <selection activeCell="J486" sqref="J486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21676,7 +21676,7 @@
       <c r="J486">
         <v>32.25</v>
       </c>
-      <c r="K486">
+      <c r="K486" s="8">
         <v>0.75</v>
       </c>
       <c r="L486">
@@ -21723,7 +21723,7 @@
       <c r="J487">
         <v>40.75</v>
       </c>
-      <c r="K487">
+      <c r="K487" s="8">
         <v>0</v>
       </c>
       <c r="L487">
@@ -21770,7 +21770,7 @@
       <c r="J488">
         <v>0</v>
       </c>
-      <c r="K488">
+      <c r="K488" s="8">
         <v>0</v>
       </c>
       <c r="L488">
@@ -21823,7 +21823,7 @@
       <c r="J489">
         <v>0</v>
       </c>
-      <c r="K489">
+      <c r="K489" s="8">
         <v>0</v>
       </c>
       <c r="L489">

</xml_diff>